<commit_message>
Add convention about JavaScript.
</commit_message>
<xml_diff>
--- a/sample-common/doc/ConventionsForScreenImplementation.xlsx
+++ b/sample-common/doc/ConventionsForScreenImplementation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26518"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="12800" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HTML" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="474">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -3804,6 +3804,175 @@
     </rPh>
     <rPh sb="12" eb="14">
       <t>メイジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DOM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>クロスプラットフォーム</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>モバイル</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>モバイル向けには使用しない</t>
+    <rPh sb="4" eb="5">
+      <t>ム</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タッチイベントの処理が300ミリ秒遅延するため、性能問題が発生する。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Clickイベントは使わず、ライラリを利用する。</t>
+    <rPh sb="10" eb="11">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>リヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>モバイル</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HTMLファイル名が表示されるため。</t>
+    <rPh sb="8" eb="9">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>alert関数、confirm関数は使用せず、ネイティブのダイアログをコールするか、HTML5で実装する。</t>
+    <rPh sb="5" eb="7">
+      <t>カンスウ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>カンスウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ジッソウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ループ内でDOM操作をしない</t>
+    <rPh sb="3" eb="4">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ソウサ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DOMの操作は高コストのため性能問題が発生する可能性がある。</t>
+    <rPh sb="4" eb="6">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>コウ</t>
+    </rPh>
+    <rPh sb="14" eb="18">
+      <t>セイノウモンダイ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ハッセイ</t>
+    </rPh>
+    <rPh sb="23" eb="26">
+      <t>カノウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>クリックイベントの処理がタッチ後、300ミリ秒遅延する(ダブルタップか判定する)ため、性能問題が発生する可能性がある。</t>
+    <rPh sb="9" eb="11">
+      <t>ショリガ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ゴ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ビョウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>チエン</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ハンテイ</t>
+    </rPh>
+    <rPh sb="43" eb="47">
+      <t>セイノウモンダイ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ハッセイ</t>
+    </rPh>
+    <rPh sb="52" eb="55">
+      <t>カノウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>以下のいずれかにより対応
+・ループ処理の外で変更処理を行う。
+・DocumentFragmentを使用する
+・DOMツリー上から一旦切り離して、処理後に戻す。</t>
+    <rPh sb="0" eb="2">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>タイオウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ソト</t>
+    </rPh>
+    <rPh sb="22" eb="26">
+      <t>ヘンコウショリ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>イッタン</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="68" eb="69">
+      <t>ハナ</t>
+    </rPh>
+    <rPh sb="72" eb="75">
+      <t>ショリゴ</t>
+    </rPh>
+    <rPh sb="76" eb="77">
+      <t>モド</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3958,7 +4127,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="433">
+  <cellStyleXfs count="435">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4392,8 +4561,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4450,8 +4621,20 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="433">
+  <cellStyles count="435">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -4668,6 +4851,7 @@
     <cellStyle name="ハイパーリンク" xfId="427" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="429" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="433" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -4885,6 +5069,7 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="428" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="430" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="434" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -5213,13 +5398,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y159"/>
+  <dimension ref="A1:Y160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="V48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y7" sqref="W1:Y7"/>
+      <selection pane="bottomRight" activeCell="X59" sqref="X59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -5401,7 +5586,7 @@
     </row>
     <row r="4" spans="1:25" ht="44">
       <c r="A4" s="5">
-        <f t="shared" ref="A4:A67" si="0">ROW()-2</f>
+        <f t="shared" ref="A4:A68" si="0">ROW()-2</f>
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -8459,58 +8644,66 @@
       <c r="X57" s="6"/>
       <c r="Y57" s="6"/>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:25" ht="31">
       <c r="A58" s="5">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>115</v>
+        <v>22</v>
       </c>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
+      <c r="L58" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="M58" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="N58" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="N58" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="O58" s="5" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="P58" s="5" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="Q58" s="5" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="R58" s="5" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="S58" s="5" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="T58" s="5" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="U58" s="5" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="V58" s="5"/>
-      <c r="W58" s="6"/>
-      <c r="X58" s="6"/>
+      <c r="W58" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="X58" s="6" t="s">
+        <v>465</v>
+      </c>
       <c r="Y58" s="6"/>
     </row>
     <row r="59" spans="1:25">
@@ -8519,10 +8712,10 @@
         <v>57</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
@@ -8532,7 +8725,7 @@
         <v>93</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
@@ -8573,10 +8766,10 @@
         <v>58</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>205</v>
+        <v>116</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
@@ -8592,7 +8785,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
       <c r="M60" s="5" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="N60" s="5"/>
       <c r="O60" s="5" t="s">
@@ -8627,26 +8820,26 @@
         <v>59</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>208</v>
+        <v>93</v>
       </c>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
       <c r="M61" s="5" t="s">
-        <v>171</v>
+        <v>117</v>
       </c>
       <c r="N61" s="5"/>
       <c r="O61" s="5" t="s">
@@ -8670,25 +8863,21 @@
       <c r="U61" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="V61" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="V61" s="5"/>
       <c r="W61" s="6"/>
       <c r="X61" s="6"/>
-      <c r="Y61" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="62" spans="1:25" ht="31">
+      <c r="Y61" s="6"/>
+    </row>
+    <row r="62" spans="1:25">
       <c r="A62" s="5">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
@@ -8728,21 +8917,25 @@
       <c r="U62" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="V62" s="5"/>
+      <c r="V62" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="W62" s="6"/>
       <c r="X62" s="6"/>
-      <c r="Y62" s="6"/>
-    </row>
-    <row r="63" spans="1:25">
+      <c r="Y62" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" ht="31">
       <c r="A63" s="5">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
@@ -8787,16 +8980,16 @@
       <c r="X63" s="6"/>
       <c r="Y63" s="6"/>
     </row>
-    <row r="64" spans="1:25" ht="31">
+    <row r="64" spans="1:25">
       <c r="A64" s="5">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
@@ -8847,10 +9040,10 @@
         <v>63</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
@@ -8895,16 +9088,16 @@
       <c r="X65" s="6"/>
       <c r="Y65" s="6"/>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" ht="31">
       <c r="A66" s="5">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
@@ -8955,10 +9148,10 @@
         <v>65</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
@@ -9005,14 +9198,14 @@
     </row>
     <row r="68" spans="1:25">
       <c r="A68" s="5">
-        <f t="shared" ref="A68:A135" si="1">ROW()-2</f>
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
@@ -9059,14 +9252,14 @@
     </row>
     <row r="69" spans="1:25">
       <c r="A69" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A69:A136" si="1">ROW()-2</f>
         <v>67</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
@@ -9117,10 +9310,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
@@ -9165,32 +9358,32 @@
       <c r="X70" s="6"/>
       <c r="Y70" s="6"/>
     </row>
-    <row r="71" spans="1:25" ht="31">
+    <row r="71" spans="1:25">
       <c r="A71" s="5">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
       <c r="H71" s="5" t="s">
-        <v>229</v>
+        <v>171</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
       <c r="M71" s="5" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="N71" s="5"/>
       <c r="O71" s="5" t="s">
@@ -9225,10 +9418,10 @@
         <v>70</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
@@ -9279,10 +9472,10 @@
         <v>71</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
@@ -9333,10 +9526,10 @@
         <v>72</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
@@ -9387,10 +9580,10 @@
         <v>73</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
@@ -9425,70 +9618,66 @@
         <v>93</v>
       </c>
       <c r="T75" s="5" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="U75" s="5" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="V75" s="5"/>
       <c r="W75" s="6"/>
       <c r="X75" s="6"/>
-      <c r="Y75" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="76" spans="1:25">
+      <c r="Y75" s="6"/>
+    </row>
+    <row r="76" spans="1:25" ht="31">
       <c r="A76" s="5">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="5" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>171</v>
+        <v>230</v>
       </c>
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
       <c r="M76" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="N76" s="5"/>
       <c r="O76" s="5" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="P76" s="5" t="s">
-        <v>175</v>
+        <v>93</v>
       </c>
       <c r="Q76" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="R76" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="S76" s="5" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="T76" s="5" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="U76" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="V76" s="5" t="s">
-        <v>171</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="V76" s="5"/>
       <c r="W76" s="6"/>
       <c r="X76" s="6"/>
       <c r="Y76" s="6" t="s">
@@ -9501,23 +9690,27 @@
         <v>75</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D77" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
+      <c r="H77" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
-      <c r="M77" s="5"/>
+      <c r="M77" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="N77" s="5"/>
       <c r="O77" s="5" t="s">
         <v>173</v>
@@ -9555,7 +9748,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>242</v>
@@ -9599,58 +9792,58 @@
       </c>
       <c r="W78" s="6"/>
       <c r="X78" s="6"/>
-      <c r="Y78" s="6"/>
-    </row>
-    <row r="79" spans="1:25" ht="31">
+      <c r="Y78" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25">
       <c r="A79" s="5">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="D79" s="5"/>
+        <v>242</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
       <c r="G79" s="5"/>
-      <c r="H79" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="I79" s="5" t="s">
-        <v>165</v>
-      </c>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
-      <c r="M79" s="5" t="s">
-        <v>255</v>
-      </c>
+      <c r="M79" s="5"/>
       <c r="N79" s="5"/>
       <c r="O79" s="5" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="P79" s="5" t="s">
-        <v>93</v>
+        <v>175</v>
       </c>
       <c r="Q79" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="R79" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="S79" s="5" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="T79" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="U79" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="V79" s="5"/>
+        <v>171</v>
+      </c>
+      <c r="V79" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="W79" s="6"/>
       <c r="X79" s="6"/>
       <c r="Y79" s="6"/>
@@ -9661,7 +9854,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>245</v>
@@ -9671,7 +9864,7 @@
       <c r="F80" s="5"/>
       <c r="G80" s="5"/>
       <c r="H80" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>165</v>
@@ -9680,33 +9873,31 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
       <c r="M80" s="5" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
       <c r="N80" s="5"/>
       <c r="O80" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="P80" s="5" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="Q80" s="5" t="s">
-        <v>249</v>
+        <v>93</v>
       </c>
       <c r="R80" s="5" t="s">
-        <v>250</v>
+        <v>93</v>
       </c>
       <c r="S80" s="5" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="T80" s="5" t="s">
-        <v>247</v>
+        <v>93</v>
       </c>
       <c r="U80" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="V80" s="5" t="s">
-        <v>165</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="V80" s="5"/>
       <c r="W80" s="6"/>
       <c r="X80" s="6"/>
       <c r="Y80" s="6"/>
@@ -9717,17 +9908,17 @@
         <v>79</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
       <c r="H81" s="5" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>165</v>
@@ -9736,33 +9927,33 @@
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
       <c r="M81" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="N81" s="5" t="s">
         <v>165</v>
       </c>
+      <c r="N81" s="5"/>
       <c r="O81" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="P81" s="5" t="s">
-        <v>93</v>
+        <v>165</v>
       </c>
       <c r="Q81" s="5" t="s">
-        <v>93</v>
+        <v>249</v>
       </c>
       <c r="R81" s="5" t="s">
-        <v>93</v>
+        <v>250</v>
       </c>
       <c r="S81" s="5" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="T81" s="5" t="s">
-        <v>93</v>
+        <v>247</v>
       </c>
       <c r="U81" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="V81" s="5"/>
+        <v>248</v>
+      </c>
+      <c r="V81" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="W81" s="6"/>
       <c r="X81" s="6"/>
       <c r="Y81" s="6"/>
@@ -9773,10 +9964,10 @@
         <v>80</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
@@ -9792,10 +9983,10 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
       <c r="M82" s="5" t="s">
-        <v>171</v>
+        <v>255</v>
       </c>
       <c r="N82" s="5" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="O82" s="5" t="s">
         <v>93</v>
@@ -9823,32 +10014,36 @@
       <c r="X82" s="6"/>
       <c r="Y82" s="6"/>
     </row>
-    <row r="83" spans="1:25">
+    <row r="83" spans="1:25" ht="31">
       <c r="A83" s="5">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J83" s="5"/>
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
-      <c r="M83" s="5"/>
-      <c r="N83" s="5"/>
+      <c r="M83" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="N83" s="5" t="s">
+        <v>175</v>
+      </c>
       <c r="O83" s="5" t="s">
         <v>93</v>
       </c>
@@ -9875,16 +10070,16 @@
       <c r="X83" s="6"/>
       <c r="Y83" s="6"/>
     </row>
-    <row r="84" spans="1:25" ht="31">
+    <row r="84" spans="1:25">
       <c r="A84" s="5">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
@@ -9894,7 +10089,7 @@
         <v>171</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
@@ -9922,25 +10117,21 @@
       <c r="U84" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="V84" s="5" t="s">
-        <v>165</v>
-      </c>
+      <c r="V84" s="5"/>
       <c r="W84" s="6"/>
       <c r="X84" s="6"/>
-      <c r="Y84" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="85" spans="1:25" ht="44">
+      <c r="Y84" s="6"/>
+    </row>
+    <row r="85" spans="1:25" ht="31">
       <c r="A85" s="5">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
@@ -9949,13 +10140,13 @@
       <c r="H85" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="I85" s="5"/>
+      <c r="I85" s="5" t="s">
+        <v>175</v>
+      </c>
       <c r="J85" s="5"/>
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
-      <c r="M85" s="5" t="s">
-        <v>268</v>
-      </c>
+      <c r="M85" s="5"/>
       <c r="N85" s="5"/>
       <c r="O85" s="5" t="s">
         <v>93</v>
@@ -9978,38 +10169,40 @@
       <c r="U85" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="V85" s="5"/>
-      <c r="W85" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="X85" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y85" s="6"/>
-    </row>
-    <row r="86" spans="1:25" ht="31">
+      <c r="V85" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="W85" s="6"/>
+      <c r="X85" s="6"/>
+      <c r="Y85" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25" ht="44">
       <c r="A86" s="5">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>171</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="D86" s="5"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
-      <c r="H86" s="5"/>
+      <c r="H86" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="I86" s="5"/>
       <c r="J86" s="5"/>
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
-      <c r="M86" s="5"/>
+      <c r="M86" s="5" t="s">
+        <v>268</v>
+      </c>
       <c r="N86" s="5"/>
       <c r="O86" s="5" t="s">
         <v>93</v>
@@ -10034,23 +10227,23 @@
       </c>
       <c r="V86" s="5"/>
       <c r="W86" s="6" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="X86" s="6" t="s">
         <v>98</v>
       </c>
       <c r="Y86" s="6"/>
     </row>
-    <row r="87" spans="1:25" ht="44">
+    <row r="87" spans="1:25" ht="31">
       <c r="A87" s="5">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>171</v>
@@ -10088,7 +10281,7 @@
       </c>
       <c r="V87" s="5"/>
       <c r="W87" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="X87" s="6" t="s">
         <v>98</v>
@@ -10101,13 +10294,13 @@
         <v>86</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>269</v>
+        <v>171</v>
       </c>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
@@ -10142,26 +10335,26 @@
       </c>
       <c r="V88" s="5"/>
       <c r="W88" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="X88" s="6" t="s">
         <v>98</v>
       </c>
       <c r="Y88" s="6"/>
     </row>
-    <row r="89" spans="1:25" ht="31">
+    <row r="89" spans="1:25" ht="44">
       <c r="A89" s="5">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>165</v>
+        <v>269</v>
       </c>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
@@ -10195,23 +10388,27 @@
         <v>93</v>
       </c>
       <c r="V89" s="5"/>
-      <c r="W89" s="6"/>
-      <c r="X89" s="6"/>
+      <c r="W89" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="X89" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="Y89" s="6"/>
     </row>
-    <row r="90" spans="1:25">
+    <row r="90" spans="1:25" ht="31">
       <c r="A90" s="5">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
@@ -10255,13 +10452,13 @@
         <v>89</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>277</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>279</v>
+        <v>171</v>
       </c>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
@@ -10305,13 +10502,13 @@
         <v>90</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
       <c r="E92" s="5"/>
       <c r="F92" s="5"/>
@@ -10355,7 +10552,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>283</v>
@@ -10405,13 +10602,13 @@
         <v>92</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>283</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>284</v>
+        <v>171</v>
       </c>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
@@ -10449,31 +10646,29 @@
       <c r="X94" s="6"/>
       <c r="Y94" s="6"/>
     </row>
-    <row r="95" spans="1:25" ht="31">
+    <row r="95" spans="1:25">
       <c r="A95" s="5">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="D95" s="5"/>
+        <v>283</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>284</v>
+      </c>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
-      <c r="H95" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="H95" s="5"/>
       <c r="I95" s="5"/>
       <c r="J95" s="5"/>
       <c r="K95" s="5"/>
       <c r="L95" s="5"/>
-      <c r="M95" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="M95" s="5"/>
       <c r="N95" s="5"/>
       <c r="O95" s="5" t="s">
         <v>93</v>
@@ -10497,12 +10692,8 @@
         <v>93</v>
       </c>
       <c r="V95" s="5"/>
-      <c r="W95" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="X95" s="6" t="s">
-        <v>98</v>
-      </c>
+      <c r="W95" s="6"/>
+      <c r="X95" s="6"/>
       <c r="Y95" s="6"/>
     </row>
     <row r="96" spans="1:25" ht="31">
@@ -10511,10 +10702,10 @@
         <v>94</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
@@ -10523,16 +10714,12 @@
       <c r="H96" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="I96" s="5" t="s">
-        <v>290</v>
-      </c>
+      <c r="I96" s="5"/>
       <c r="J96" s="5"/>
       <c r="K96" s="5"/>
-      <c r="L96" s="5" t="s">
-        <v>175</v>
-      </c>
+      <c r="L96" s="5"/>
       <c r="M96" s="5" t="s">
-        <v>291</v>
+        <v>171</v>
       </c>
       <c r="N96" s="5"/>
       <c r="O96" s="5" t="s">
@@ -10557,8 +10744,12 @@
         <v>93</v>
       </c>
       <c r="V96" s="5"/>
-      <c r="W96" s="6"/>
-      <c r="X96" s="6"/>
+      <c r="W96" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="X96" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="Y96" s="6"/>
     </row>
     <row r="97" spans="1:25" ht="31">
@@ -10567,48 +10758,50 @@
         <v>95</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D97" s="5"/>
-      <c r="E97" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="E97" s="5"/>
       <c r="F97" s="5"/>
       <c r="G97" s="5"/>
       <c r="H97" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="I97" s="5"/>
+      <c r="I97" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="J97" s="5"/>
       <c r="K97" s="5"/>
-      <c r="L97" s="5"/>
+      <c r="L97" s="5" t="s">
+        <v>175</v>
+      </c>
       <c r="M97" s="5" t="s">
-        <v>171</v>
+        <v>291</v>
       </c>
       <c r="N97" s="5"/>
       <c r="O97" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="P97" s="5" t="s">
-        <v>293</v>
+        <v>93</v>
       </c>
       <c r="Q97" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="R97" s="5" t="s">
-        <v>163</v>
+        <v>93</v>
       </c>
       <c r="S97" s="5" t="s">
-        <v>163</v>
+        <v>93</v>
       </c>
       <c r="T97" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="U97" s="5" t="s">
-        <v>163</v>
+        <v>93</v>
       </c>
       <c r="V97" s="5"/>
       <c r="W97" s="6"/>
@@ -10621,23 +10814,27 @@
         <v>96</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E98" s="5"/>
+        <v>294</v>
+      </c>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
-      <c r="H98" s="5"/>
+      <c r="H98" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="I98" s="5"/>
       <c r="J98" s="5"/>
       <c r="K98" s="5"/>
       <c r="L98" s="5"/>
-      <c r="M98" s="5"/>
+      <c r="M98" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="N98" s="5"/>
       <c r="O98" s="5" t="s">
         <v>171</v>
@@ -10661,12 +10858,8 @@
         <v>163</v>
       </c>
       <c r="V98" s="5"/>
-      <c r="W98" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="X98" s="6" t="s">
-        <v>98</v>
-      </c>
+      <c r="W98" s="6"/>
+      <c r="X98" s="6"/>
       <c r="Y98" s="6"/>
     </row>
     <row r="99" spans="1:25" ht="31">
@@ -10675,31 +10868,29 @@
         <v>97</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>339</v>
+        <v>295</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="D99" s="5"/>
+        <v>296</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
       <c r="G99" s="5"/>
-      <c r="H99" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="I99" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="H99" s="5"/>
+      <c r="I99" s="5"/>
       <c r="J99" s="5"/>
       <c r="K99" s="5"/>
       <c r="L99" s="5"/>
       <c r="M99" s="5"/>
       <c r="N99" s="5"/>
       <c r="O99" s="5" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="P99" s="5" t="s">
-        <v>171</v>
+        <v>293</v>
       </c>
       <c r="Q99" s="5" t="s">
         <v>171</v>
@@ -10708,7 +10899,7 @@
         <v>163</v>
       </c>
       <c r="S99" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="T99" s="5" t="s">
         <v>171</v>
@@ -10718,22 +10909,20 @@
       </c>
       <c r="V99" s="5"/>
       <c r="W99" s="6" t="s">
-        <v>340</v>
+        <v>297</v>
       </c>
       <c r="X99" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="Y99" s="6" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="100" spans="1:25">
+        <v>98</v>
+      </c>
+      <c r="Y99" s="6"/>
+    </row>
+    <row r="100" spans="1:25" ht="31">
       <c r="A100" s="5">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>298</v>
@@ -10763,7 +10952,7 @@
         <v>171</v>
       </c>
       <c r="R100" s="5" t="s">
-        <v>344</v>
+        <v>163</v>
       </c>
       <c r="S100" s="5" t="s">
         <v>171</v>
@@ -10774,12 +10963,16 @@
       <c r="U100" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="V100" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="W100" s="6"/>
-      <c r="X100" s="6"/>
-      <c r="Y100" s="6"/>
+      <c r="V100" s="5"/>
+      <c r="W100" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="X100" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="Y100" s="6" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="101" spans="1:25">
       <c r="A101" s="5">
@@ -10787,7 +10980,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>298</v>
@@ -10808,7 +11001,7 @@
       <c r="M101" s="5"/>
       <c r="N101" s="5"/>
       <c r="O101" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="P101" s="5" t="s">
         <v>171</v>
@@ -10817,7 +11010,7 @@
         <v>171</v>
       </c>
       <c r="R101" s="5" t="s">
-        <v>171</v>
+        <v>344</v>
       </c>
       <c r="S101" s="5" t="s">
         <v>171</v>
@@ -10826,7 +11019,7 @@
         <v>171</v>
       </c>
       <c r="U101" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="V101" s="5" t="s">
         <v>171</v>
@@ -10841,7 +11034,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>298</v>
@@ -10887,9 +11080,7 @@
       </c>
       <c r="W102" s="6"/>
       <c r="X102" s="6"/>
-      <c r="Y102" s="6" t="s">
-        <v>347</v>
-      </c>
+      <c r="Y102" s="6"/>
     </row>
     <row r="103" spans="1:25">
       <c r="A103" s="5">
@@ -10897,7 +11088,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>298</v>
@@ -10943,7 +11134,9 @@
       </c>
       <c r="W103" s="6"/>
       <c r="X103" s="6"/>
-      <c r="Y103" s="6"/>
+      <c r="Y103" s="6" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="104" spans="1:25">
       <c r="A104" s="5">
@@ -10951,7 +11144,7 @@
         <v>102</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>298</v>
@@ -10992,7 +11185,9 @@
       <c r="U104" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="V104" s="5"/>
+      <c r="V104" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="W104" s="6"/>
       <c r="X104" s="6"/>
       <c r="Y104" s="6"/>
@@ -11003,7 +11198,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>298</v>
@@ -11024,35 +11219,29 @@
       <c r="M105" s="5"/>
       <c r="N105" s="5"/>
       <c r="O105" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P105" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Q105" s="5" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="R105" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S105" s="5" t="s">
         <v>171</v>
       </c>
       <c r="T105" s="5" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="U105" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="V105" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="W105" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="X105" s="6" t="s">
-        <v>335</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="V105" s="5"/>
+      <c r="W105" s="6"/>
+      <c r="X105" s="6"/>
       <c r="Y105" s="6"/>
     </row>
     <row r="106" spans="1:25">
@@ -11061,7 +11250,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>298</v>
@@ -11119,7 +11308,7 @@
         <v>105</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>298</v>
@@ -11177,7 +11366,7 @@
         <v>106</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>298</v>
@@ -11235,7 +11424,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C109" s="6" t="s">
         <v>298</v>
@@ -11293,7 +11482,7 @@
         <v>108</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>298</v>
@@ -11351,7 +11540,7 @@
         <v>109</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>298</v>
@@ -11372,31 +11561,35 @@
       <c r="M111" s="5"/>
       <c r="N111" s="5"/>
       <c r="O111" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="P111" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="Q111" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="R111" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="S111" s="5" t="s">
         <v>171</v>
       </c>
       <c r="T111" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="U111" s="5" t="s">
-        <v>171</v>
+        <v>356</v>
       </c>
       <c r="V111" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="W111" s="6"/>
-      <c r="X111" s="6"/>
+      <c r="W111" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="X111" s="6" t="s">
+        <v>335</v>
+      </c>
       <c r="Y111" s="6"/>
     </row>
     <row r="112" spans="1:25">
@@ -11405,7 +11598,7 @@
         <v>110</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>298</v>
@@ -11459,7 +11652,7 @@
         <v>111</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>337</v>
+        <v>365</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>298</v>
@@ -11500,7 +11693,9 @@
       <c r="U113" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="V113" s="5"/>
+      <c r="V113" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="W113" s="6"/>
       <c r="X113" s="6"/>
       <c r="Y113" s="6"/>
@@ -11511,7 +11706,7 @@
         <v>112</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>359</v>
+        <v>337</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>298</v>
@@ -11563,7 +11758,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>338</v>
+        <v>359</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>298</v>
@@ -11584,35 +11779,29 @@
       <c r="M115" s="5"/>
       <c r="N115" s="5"/>
       <c r="O115" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P115" s="5" t="s">
-        <v>358</v>
+        <v>171</v>
       </c>
       <c r="Q115" s="5" t="s">
         <v>171</v>
       </c>
       <c r="R115" s="5" t="s">
-        <v>358</v>
+        <v>171</v>
       </c>
       <c r="S115" s="5" t="s">
         <v>171</v>
       </c>
       <c r="T115" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="U115" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="V115" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="W115" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="X115" s="6" t="s">
-        <v>335</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="V115" s="5"/>
+      <c r="W115" s="6"/>
+      <c r="X115" s="6"/>
       <c r="Y115" s="6"/>
     </row>
     <row r="116" spans="1:25">
@@ -11621,7 +11810,7 @@
         <v>114</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>360</v>
+        <v>338</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>298</v>
@@ -11642,32 +11831,36 @@
       <c r="M116" s="5"/>
       <c r="N116" s="5"/>
       <c r="O116" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="P116" s="5" t="s">
-        <v>171</v>
+        <v>358</v>
       </c>
       <c r="Q116" s="5" t="s">
         <v>171</v>
       </c>
       <c r="R116" s="5" t="s">
-        <v>171</v>
+        <v>358</v>
       </c>
       <c r="S116" s="5" t="s">
         <v>171</v>
       </c>
       <c r="T116" s="5" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="U116" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="V116" s="5"/>
-      <c r="W116" s="6"/>
-      <c r="X116" s="6"/>
-      <c r="Y116" s="6" t="s">
-        <v>361</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="V116" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="W116" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="X116" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="Y116" s="6"/>
     </row>
     <row r="117" spans="1:25">
       <c r="A117" s="5">
@@ -11675,7 +11868,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>298</v>
@@ -11711,15 +11904,17 @@
         <v>171</v>
       </c>
       <c r="T117" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="U117" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="V117" s="5"/>
       <c r="W117" s="6"/>
       <c r="X117" s="6"/>
-      <c r="Y117" s="6"/>
+      <c r="Y117" s="6" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="118" spans="1:25">
       <c r="A118" s="5">
@@ -11727,7 +11922,7 @@
         <v>116</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>336</v>
+        <v>362</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>298</v>
@@ -11779,7 +11974,7 @@
         <v>117</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>363</v>
+        <v>336</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>298</v>
@@ -11831,7 +12026,7 @@
         <v>118</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>298</v>
@@ -11883,10 +12078,10 @@
         <v>119</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>299</v>
+        <v>364</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D121" s="5"/>
       <c r="E121" s="5"/>
@@ -11901,62 +12096,58 @@
       <c r="J121" s="5"/>
       <c r="K121" s="5"/>
       <c r="L121" s="5"/>
-      <c r="M121" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="M121" s="5"/>
       <c r="N121" s="5"/>
       <c r="O121" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="P121" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="Q121" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="R121" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="S121" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="T121" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="U121" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="V121" s="5"/>
       <c r="W121" s="6"/>
       <c r="X121" s="6"/>
       <c r="Y121" s="6"/>
     </row>
-    <row r="122" spans="1:25" ht="31">
+    <row r="122" spans="1:25">
       <c r="A122" s="5">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D122" s="5"/>
       <c r="E122" s="5"/>
       <c r="F122" s="5"/>
       <c r="G122" s="5"/>
       <c r="H122" s="5" t="s">
-        <v>303</v>
+        <v>171</v>
       </c>
       <c r="I122" s="5" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="J122" s="5"/>
       <c r="K122" s="5"/>
-      <c r="L122" s="5" t="s">
-        <v>175</v>
-      </c>
+      <c r="L122" s="5"/>
       <c r="M122" s="5" t="s">
         <v>171</v>
       </c>
@@ -11993,23 +12184,29 @@
         <v>121</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="D123" s="5" t="s">
-        <v>165</v>
-      </c>
+      <c r="D123" s="5"/>
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
       <c r="G123" s="5"/>
-      <c r="H123" s="5"/>
-      <c r="I123" s="5"/>
+      <c r="H123" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="I123" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="J123" s="5"/>
       <c r="K123" s="5"/>
-      <c r="L123" s="5"/>
-      <c r="M123" s="5"/>
+      <c r="L123" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="M123" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="N123" s="5"/>
       <c r="O123" s="5" t="s">
         <v>93</v>
@@ -12043,7 +12240,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C124" s="6" t="s">
         <v>304</v>
@@ -12087,112 +12284,106 @@
       <c r="X124" s="6"/>
       <c r="Y124" s="6"/>
     </row>
-    <row r="125" spans="1:25">
+    <row r="125" spans="1:25" ht="31">
       <c r="A125" s="5">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="D125" s="5"/>
+        <v>304</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
       <c r="G125" s="5"/>
-      <c r="H125" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="I125" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="H125" s="5"/>
+      <c r="I125" s="5"/>
       <c r="J125" s="5"/>
       <c r="K125" s="5"/>
       <c r="L125" s="5"/>
       <c r="M125" s="5"/>
       <c r="N125" s="5"/>
       <c r="O125" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="P125" s="5" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="Q125" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="R125" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="S125" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="T125" s="5" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="U125" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="V125" s="5" t="s">
-        <v>171</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="V125" s="5"/>
       <c r="W125" s="6"/>
       <c r="X125" s="6"/>
       <c r="Y125" s="6"/>
     </row>
-    <row r="126" spans="1:25" ht="31">
+    <row r="126" spans="1:25">
       <c r="A126" s="5">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D126" s="5"/>
       <c r="E126" s="5"/>
       <c r="F126" s="5"/>
       <c r="G126" s="5"/>
       <c r="H126" s="5" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="I126" s="5" t="s">
         <v>171</v>
       </c>
       <c r="J126" s="5"/>
       <c r="K126" s="5"/>
-      <c r="L126" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="M126" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="L126" s="5"/>
+      <c r="M126" s="5"/>
       <c r="N126" s="5"/>
       <c r="O126" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="P126" s="5" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="Q126" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="R126" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="S126" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="T126" s="5" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="U126" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="V126" s="5"/>
+        <v>173</v>
+      </c>
+      <c r="V126" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="W126" s="6"/>
       <c r="X126" s="6"/>
       <c r="Y126" s="6"/>
@@ -12203,17 +12394,17 @@
         <v>125</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D127" s="5"/>
       <c r="E127" s="5"/>
       <c r="F127" s="5"/>
       <c r="G127" s="5"/>
       <c r="H127" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I127" s="5" t="s">
         <v>171</v>
@@ -12221,50 +12412,48 @@
       <c r="J127" s="5"/>
       <c r="K127" s="5"/>
       <c r="L127" s="5" t="s">
-        <v>311</v>
+        <v>165</v>
       </c>
       <c r="M127" s="5" t="s">
         <v>171</v>
       </c>
       <c r="N127" s="5"/>
       <c r="O127" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="P127" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="Q127" s="5" t="s">
-        <v>311</v>
+        <v>93</v>
       </c>
       <c r="R127" s="5" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="S127" s="5" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="T127" s="5" t="s">
-        <v>173</v>
+        <v>93</v>
       </c>
       <c r="U127" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="V127" s="5" t="s">
-        <v>171</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="V127" s="5"/>
       <c r="W127" s="6"/>
       <c r="X127" s="6"/>
       <c r="Y127" s="6"/>
     </row>
-    <row r="128" spans="1:25">
+    <row r="128" spans="1:25" ht="31">
       <c r="A128" s="5">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D128" s="5"/>
       <c r="E128" s="5"/>
@@ -12278,63 +12467,61 @@
       </c>
       <c r="J128" s="5"/>
       <c r="K128" s="5"/>
-      <c r="L128" s="5"/>
+      <c r="L128" s="5" t="s">
+        <v>311</v>
+      </c>
       <c r="M128" s="5" t="s">
         <v>171</v>
       </c>
       <c r="N128" s="5"/>
       <c r="O128" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="P128" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="Q128" s="5" t="s">
-        <v>93</v>
+        <v>311</v>
       </c>
       <c r="R128" s="5" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="S128" s="5" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="T128" s="5" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="U128" s="5" t="s">
-        <v>93</v>
+        <v>312</v>
       </c>
       <c r="V128" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="W128" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="X128" s="6" t="s">
-        <v>335</v>
-      </c>
+      <c r="W128" s="6"/>
+      <c r="X128" s="6"/>
       <c r="Y128" s="6"/>
     </row>
-    <row r="129" spans="1:25" ht="31">
+    <row r="129" spans="1:25">
       <c r="A129" s="5">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D129" s="5"/>
       <c r="E129" s="5"/>
       <c r="F129" s="5"/>
       <c r="G129" s="5"/>
       <c r="H129" s="5" t="s">
-        <v>318</v>
+        <v>171</v>
       </c>
       <c r="I129" s="5" t="s">
-        <v>303</v>
+        <v>171</v>
       </c>
       <c r="J129" s="5"/>
       <c r="K129" s="5"/>
@@ -12344,43 +12531,47 @@
       </c>
       <c r="N129" s="5"/>
       <c r="O129" s="5" t="s">
-        <v>318</v>
+        <v>93</v>
       </c>
       <c r="P129" s="5" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="Q129" s="5" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="R129" s="5" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="S129" s="5" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="T129" s="5" t="s">
-        <v>250</v>
+        <v>93</v>
       </c>
       <c r="U129" s="5" t="s">
-        <v>250</v>
+        <v>93</v>
       </c>
       <c r="V129" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="W129" s="6"/>
-      <c r="X129" s="6"/>
+        <v>171</v>
+      </c>
+      <c r="W129" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="X129" s="6" t="s">
+        <v>335</v>
+      </c>
       <c r="Y129" s="6"/>
     </row>
-    <row r="130" spans="1:25">
+    <row r="130" spans="1:25" ht="31">
       <c r="A130" s="5">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D130" s="5"/>
       <c r="E130" s="5"/>
@@ -12390,7 +12581,7 @@
         <v>318</v>
       </c>
       <c r="I130" s="5" t="s">
-        <v>171</v>
+        <v>303</v>
       </c>
       <c r="J130" s="5"/>
       <c r="K130" s="5"/>
@@ -12400,86 +12591,84 @@
       </c>
       <c r="N130" s="5"/>
       <c r="O130" s="5" t="s">
-        <v>171</v>
+        <v>318</v>
       </c>
       <c r="P130" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="Q130" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="R130" s="5" t="s">
-        <v>321</v>
+        <v>165</v>
       </c>
       <c r="S130" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="T130" s="5" t="s">
-        <v>173</v>
+        <v>250</v>
       </c>
       <c r="U130" s="5" t="s">
-        <v>173</v>
+        <v>250</v>
       </c>
       <c r="V130" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="W130" s="6"/>
       <c r="X130" s="6"/>
       <c r="Y130" s="6"/>
     </row>
-    <row r="131" spans="1:25" ht="31">
+    <row r="131" spans="1:25">
       <c r="A131" s="5">
         <f t="shared" si="1"/>
         <v>129</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D131" s="5"/>
-      <c r="E131" s="5" t="s">
-        <v>165</v>
-      </c>
+      <c r="E131" s="5"/>
       <c r="F131" s="5"/>
       <c r="G131" s="5"/>
       <c r="H131" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="I131" s="5"/>
+        <v>318</v>
+      </c>
+      <c r="I131" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="J131" s="5"/>
       <c r="K131" s="5"/>
-      <c r="L131" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="L131" s="5"/>
       <c r="M131" s="5" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="N131" s="5"/>
       <c r="O131" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="P131" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q131" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="R131" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="S131" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="T131" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="P131" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="Q131" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="R131" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="S131" s="5" t="s">
+      <c r="U131" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="T131" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="U131" s="5" t="s">
-        <v>175</v>
-      </c>
       <c r="V131" s="5" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="W131" s="6"/>
       <c r="X131" s="6"/>
@@ -12491,23 +12680,29 @@
         <v>130</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C132" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="D132" s="5" t="s">
+      <c r="D132" s="5"/>
+      <c r="E132" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="E132" s="5"/>
       <c r="F132" s="5"/>
       <c r="G132" s="5"/>
-      <c r="H132" s="5"/>
+      <c r="H132" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="I132" s="5"/>
       <c r="J132" s="5"/>
       <c r="K132" s="5"/>
-      <c r="L132" s="5"/>
-      <c r="M132" s="5"/>
+      <c r="L132" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="M132" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="N132" s="5"/>
       <c r="O132" s="5" t="s">
         <v>173</v>
@@ -12543,56 +12738,50 @@
         <v>131</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="D133" s="5"/>
+        <v>323</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="E133" s="5"/>
       <c r="F133" s="5"/>
       <c r="G133" s="5"/>
-      <c r="H133" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="H133" s="5"/>
       <c r="I133" s="5"/>
       <c r="J133" s="5"/>
       <c r="K133" s="5"/>
-      <c r="L133" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="M133" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="L133" s="5"/>
+      <c r="M133" s="5"/>
       <c r="N133" s="5"/>
       <c r="O133" s="5" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="P133" s="5" t="s">
-        <v>163</v>
+        <v>324</v>
       </c>
       <c r="Q133" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="R133" s="5" t="s">
-        <v>163</v>
+        <v>250</v>
       </c>
       <c r="S133" s="5" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="T133" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="U133" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="V133" s="5"/>
-      <c r="W133" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="X133" s="6" t="s">
-        <v>335</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="V133" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="W133" s="6"/>
+      <c r="X133" s="6"/>
       <c r="Y133" s="6"/>
     </row>
     <row r="134" spans="1:25" ht="31">
@@ -12601,7 +12790,7 @@
         <v>132</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C134" s="6" t="s">
         <v>328</v>
@@ -12609,19 +12798,19 @@
       <c r="D134" s="5"/>
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
-      <c r="G134" s="5" t="s">
-        <v>175</v>
-      </c>
+      <c r="G134" s="5"/>
       <c r="H134" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="I134" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="I134" s="5"/>
       <c r="J134" s="5"/>
       <c r="K134" s="5"/>
-      <c r="L134" s="5"/>
-      <c r="M134" s="5"/>
+      <c r="L134" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="M134" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="N134" s="5"/>
       <c r="O134" s="5" t="s">
         <v>163</v>
@@ -12644,9 +12833,7 @@
       <c r="U134" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="V134" s="5" t="s">
-        <v>329</v>
-      </c>
+      <c r="V134" s="5"/>
       <c r="W134" s="6" t="s">
         <v>330</v>
       </c>
@@ -12655,55 +12842,57 @@
       </c>
       <c r="Y134" s="6"/>
     </row>
-    <row r="135" spans="1:25">
+    <row r="135" spans="1:25" ht="31">
       <c r="A135" s="5">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D135" s="5"/>
-      <c r="E135" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="E135" s="5"/>
       <c r="F135" s="5"/>
-      <c r="G135" s="5"/>
+      <c r="G135" s="5" t="s">
+        <v>175</v>
+      </c>
       <c r="H135" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="I135" s="5"/>
+      <c r="I135" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="J135" s="5"/>
       <c r="K135" s="5"/>
       <c r="L135" s="5"/>
       <c r="M135" s="5"/>
       <c r="N135" s="5"/>
       <c r="O135" s="5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="P135" s="5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="Q135" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="R135" s="5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="S135" s="5" t="s">
-        <v>333</v>
+        <v>163</v>
       </c>
       <c r="T135" s="5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="U135" s="5" t="s">
-        <v>333</v>
+        <v>163</v>
       </c>
       <c r="V135" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="W135" s="6" t="s">
         <v>330</v>
@@ -12714,30 +12903,61 @@
       <c r="Y135" s="6"/>
     </row>
     <row r="136" spans="1:25">
-      <c r="A136" s="5"/>
-      <c r="B136" s="5"/>
-      <c r="C136" s="6"/>
+      <c r="A136" s="5">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>332</v>
+      </c>
       <c r="D136" s="5"/>
-      <c r="E136" s="5"/>
+      <c r="E136" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="F136" s="5"/>
       <c r="G136" s="5"/>
-      <c r="H136" s="5"/>
+      <c r="H136" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="I136" s="5"/>
       <c r="J136" s="5"/>
       <c r="K136" s="5"/>
       <c r="L136" s="5"/>
       <c r="M136" s="5"/>
       <c r="N136" s="5"/>
-      <c r="O136" s="5"/>
-      <c r="P136" s="5"/>
-      <c r="Q136" s="5"/>
-      <c r="R136" s="5"/>
-      <c r="S136" s="5"/>
-      <c r="T136" s="5"/>
-      <c r="U136" s="5"/>
-      <c r="V136" s="5"/>
-      <c r="W136" s="6"/>
-      <c r="X136" s="6"/>
+      <c r="O136" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="P136" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q136" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="R136" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="S136" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="T136" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="U136" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="V136" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="W136" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="X136" s="6" t="s">
+        <v>335</v>
+      </c>
       <c r="Y136" s="6"/>
     </row>
     <row r="137" spans="1:25">
@@ -13360,6 +13580,33 @@
       <c r="W159" s="6"/>
       <c r="X159" s="6"/>
       <c r="Y159" s="6"/>
+    </row>
+    <row r="160" spans="1:25">
+      <c r="A160" s="5"/>
+      <c r="B160" s="5"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="5"/>
+      <c r="F160" s="5"/>
+      <c r="G160" s="5"/>
+      <c r="H160" s="5"/>
+      <c r="I160" s="5"/>
+      <c r="J160" s="5"/>
+      <c r="K160" s="5"/>
+      <c r="L160" s="5"/>
+      <c r="M160" s="5"/>
+      <c r="N160" s="5"/>
+      <c r="O160" s="5"/>
+      <c r="P160" s="5"/>
+      <c r="Q160" s="5"/>
+      <c r="R160" s="5"/>
+      <c r="S160" s="5"/>
+      <c r="T160" s="5"/>
+      <c r="U160" s="5"/>
+      <c r="V160" s="5"/>
+      <c r="W160" s="6"/>
+      <c r="X160" s="6"/>
+      <c r="Y160" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -13388,8 +13635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -14413,7 +14660,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -14422,7 +14669,7 @@
     <col min="2" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="59.83203125" customWidth="1"/>
     <col min="5" max="5" width="57" customWidth="1"/>
-    <col min="6" max="6" width="42" customWidth="1"/>
+    <col min="6" max="6" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -14576,38 +14823,60 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="57">
       <c r="A10" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>461</v>
+      </c>
       <c r="C10" s="8"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="8">
+      <c r="D10" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="31">
+      <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="8">
+      <c r="B11" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" s="22" customFormat="1" ht="31">
+      <c r="A12" s="21">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="8"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21" t="s">
+        <v>467</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>469</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>468</v>
+      </c>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="8">

</xml_diff>